<commit_message>
Create rate card: cityone-clusterone-orgone
</commit_message>
<xml_diff>
--- a/src/main/resources/excel/hyperlocal/cityone/clusterone/orgone/CityoneClusteroneOrgone.xlsx
+++ b/src/main/resources/excel/hyperlocal/cityone/clusterone/orgone/CityoneClusteroneOrgone.xlsx
@@ -405,10 +405,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="28">
     <font>
@@ -466,9 +466,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
       <name val="Arial"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -480,23 +480,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF800080"/>
       <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -518,8 +518,24 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -527,14 +543,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -555,24 +563,39 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Arial"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF9C6500"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -586,31 +609,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFFA7D00"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -667,13 +667,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -685,7 +703,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -697,13 +715,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -715,31 +733,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -751,13 +757,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -775,13 +781,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -793,61 +835,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1025,6 +1025,30 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -1040,15 +1064,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -1060,15 +1075,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1099,123 +1105,117 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="13" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="16" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="17" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="18" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1224,40 +1224,40 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="28" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1682,8 +1682,8 @@
   <sheetPr/>
   <dimension ref="A1:AA851"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:C2"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6339285714286" defaultRowHeight="15" customHeight="1"/>
@@ -1705,7 +1705,7 @@
     <col min="15" max="15" width="24.6428571428571" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" outlineLevel="1" spans="1:3">
+    <row r="1" ht="12" outlineLevel="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2024,7 +2024,7 @@
       <c r="G17" s="35"/>
       <c r="H17" s="55"/>
       <c r="I17" s="55">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="J17" s="35"/>
       <c r="K17" s="35"/>
@@ -2043,7 +2043,7 @@
       <c r="G18" s="35"/>
       <c r="H18" s="55"/>
       <c r="I18" s="55">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="J18" s="35" t="s">
         <v>35</v>

</xml_diff>

<commit_message>
Create rate card: cityone-clusterone-orgone (#14)
</commit_message>
<xml_diff>
--- a/src/main/resources/excel/hyperlocal/cityone/clusterone/orgone/CityoneClusteroneOrgone.xlsx
+++ b/src/main/resources/excel/hyperlocal/cityone/clusterone/orgone/CityoneClusteroneOrgone.xlsx
@@ -405,10 +405,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="28">
     <font>
@@ -466,9 +466,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
       <name val="Arial"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -480,23 +480,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF800080"/>
       <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -518,8 +518,24 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -527,14 +543,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -555,24 +563,39 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Arial"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF9C6500"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -586,31 +609,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFFA7D00"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -667,13 +667,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -685,7 +703,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -697,13 +715,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -715,31 +733,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -751,13 +757,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -775,13 +781,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -793,61 +835,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1025,6 +1025,30 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -1040,15 +1064,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -1060,15 +1075,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1099,123 +1105,117 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="13" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="16" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="17" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="18" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1224,40 +1224,40 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="28" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1682,8 +1682,8 @@
   <sheetPr/>
   <dimension ref="A1:AA851"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:C2"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6339285714286" defaultRowHeight="15" customHeight="1"/>
@@ -1705,7 +1705,7 @@
     <col min="15" max="15" width="24.6428571428571" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" outlineLevel="1" spans="1:3">
+    <row r="1" ht="12" outlineLevel="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2024,7 +2024,7 @@
       <c r="G17" s="35"/>
       <c r="H17" s="55"/>
       <c r="I17" s="55">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="J17" s="35"/>
       <c r="K17" s="35"/>
@@ -2043,7 +2043,7 @@
       <c r="G18" s="35"/>
       <c r="H18" s="55"/>
       <c r="I18" s="55">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="J18" s="35" t="s">
         <v>35</v>

</xml_diff>